<commit_message>
Adding Web Table files
</commit_message>
<xml_diff>
--- a/Python_Selenium/test_data/DEMOQA.xlsx
+++ b/Python_Selenium/test_data/DEMOQA.xlsx
@@ -1,41 +1,126 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse\eclipse-jee-2023-03-R-win32-x86_64\API\Python_Selenium\test_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CAD70F-C57E-4822-81E3-729D3ACF63F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DEMOQA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DEMOQA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>Sherki</t>
+  </si>
+  <si>
+    <t>sachin@gmail.com</t>
+  </si>
+  <si>
+    <t>Quality Analyst</t>
+  </si>
+  <si>
+    <t>Pratik</t>
+  </si>
+  <si>
+    <t>Yewale</t>
+  </si>
+  <si>
+    <t>pratik@gmail.com</t>
+  </si>
+  <si>
+    <t>System Engineer</t>
+  </si>
+  <si>
+    <t>Ashish</t>
+  </si>
+  <si>
+    <t>Sonar</t>
+  </si>
+  <si>
+    <t>ashish@gmail.com</t>
+  </si>
+  <si>
+    <t>Designer Civil</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Phavade</t>
+  </si>
+  <si>
+    <t>rahul@gmail.com</t>
+  </si>
+  <si>
+    <t>Omkar</t>
+  </si>
+  <si>
+    <t>Meshram</t>
+  </si>
+  <si>
+    <t>omkar@gmail.com</t>
+  </si>
+  <si>
+    <t>Automation Engineer</t>
+  </si>
+  <si>
+    <t>userEmail</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,89 +161,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -458,206 +484,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="9.77734375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.6640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="16.44140625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="4" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="8" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="18.33203125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="4">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>firstname</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>lastname</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>age</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>salary</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>department</t>
-        </is>
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Sachin</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>Sherki</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>sachin@gmail.com</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
         <v>27</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="1">
         <v>1500000</v>
       </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>Quality Analyst</t>
-        </is>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Pratik</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>Yewale</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>pratik@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
         <v>26</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="1">
         <v>1500000</v>
       </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>System Engineer</t>
-        </is>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Ashish</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>Sonar</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>ashish@gmail.com</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="1">
         <v>1000000</v>
       </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>Designer Civil</t>
-        </is>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Rahul</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>Phavade</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>rahul@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="n">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1">
         <v>26</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="1">
         <v>1200000</v>
       </c>
-      <c r="F5" s="1" t="inlineStr">
-        <is>
-          <t>Quality Analyst</t>
-        </is>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Omkar</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>Meshram</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>omkar@gmail.com</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="n">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1">
         <v>26</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="1">
         <v>1000000</v>
       </c>
-      <c r="F6" s="1" t="inlineStr">
-        <is>
-          <t>Automation Engineer</t>
-        </is>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C6" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>